<commit_message>
cambios facturacion y contabilidad
</commit_message>
<xml_diff>
--- a/TEMP/EMPRESA_998/SubCuentas De Proyectos.xlsx
+++ b/TEMP/EMPRESA_998/SubCuentas De Proyectos.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>VACA PRIETO WALTER JALIL</t>
   </si>
@@ -42,7 +42,7 @@
         <sz val="7"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">18:24
+      <t xml:space="preserve">15:26
 </t>
     </r>
     <r>
@@ -67,7 +67,7 @@
         <sz val="7"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">05-12-2024
+      <t xml:space="preserve">13-01-2025
 </t>
     </r>
     <r>
@@ -92,7 +92,7 @@
         <sz val="7"/>
         <u val="none"/>
       </rPr>
-      <t xml:space="preserve">jean piere asencio</t>
+      <t xml:space="preserve">Vaca Prieto Walter Jalil</t>
     </r>
   </si>
   <si>
@@ -112,6 +112,48 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>1.1.03.02.10.01</t>
+  </si>
+  <si>
+    <t>MP CASA 1</t>
+  </si>
+  <si>
+    <t>Costo Administrativo</t>
+  </si>
+  <si>
+    <t>000COSTADM</t>
+  </si>
+  <si>
+    <t>1.1.03.02.10.02</t>
+  </si>
+  <si>
+    <t>MP CASA 2</t>
+  </si>
+  <si>
+    <t>Costos Financieros</t>
+  </si>
+  <si>
+    <t>000COSTFIN</t>
+  </si>
+  <si>
+    <t>1.1.03.02.10.03</t>
+  </si>
+  <si>
+    <t>MP CASA 3</t>
+  </si>
+  <si>
+    <t>ESTADO DE RESULTADO BATA</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>1.1.03.02.17.01</t>
+  </si>
+  <si>
+    <t>MP REPLANTEO</t>
   </si>
 </sst>
 </file>
@@ -566,7 +608,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="E3" sqref="E3"/>
@@ -612,7 +654,7 @@
               <sz val="7"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">18:24
+            <t xml:space="preserve">15:26
 </t>
           </r>
           <r>
@@ -637,7 +679,7 @@
               <sz val="7"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">05-12-2024
+            <t xml:space="preserve">13-01-2025
 </t>
           </r>
           <r>
@@ -662,7 +704,7 @@
               <sz val="7"/>
               <u val="none"/>
             </rPr>
-            <t xml:space="preserve">jean piere asencio</t>
+            <t xml:space="preserve">Vaca Prieto Walter Jalil</t>
           </r>
         </is>
       </c>
@@ -687,6 +729,74 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>